<commit_message>
update scripts for chapter 14
</commit_message>
<xml_diff>
--- a/Chapter13/position_data.xlsx
+++ b/Chapter13/position_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason118/PycharmProjects/selenium4.0-automation/Chapter10/Chapter10.3.2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason118/PycharmProjects/selenium4.0-automation/Chapter13/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FF8EFB-AA7B-3F47-905F-B8AFD2114C0B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92C9DE8-981C-F341-B176-CC5B1B1400D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="940" windowWidth="27640" windowHeight="15620" xr2:uid="{ED4AC1EC-C70D-D844-8266-2C2596F1EA1D}"/>
   </bookViews>
@@ -33,10 +33,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Post03052022</t>
+    <t>Post03112022</t>
   </si>
   <si>
-    <t>PostCode03052022</t>
+    <t>PostCode03112022</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>